<commit_message>
Final changes of Broken Links
</commit_message>
<xml_diff>
--- a/BrokenLink/src/main/resources/AllLinks_STG.xlsx
+++ b/BrokenLink/src/main/resources/AllLinks_STG.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="URL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>FileName</t>
   </si>
@@ -22,65 +22,12 @@
     <t>Connect</t>
   </si>
   <si>
-    <t>Inventory</t>
-  </si>
-  <si>
-    <t>Test Utility (Cheetah Order Processing
-Cheetah Track URL
-Tive
-FedEx CIL/ MDSI
-Xcel Processing
-Flight Delay/ Cancel - Manual)</t>
-  </si>
-  <si>
-    <t>DirectTaskLog</t>
-  </si>
-  <si>
-    <t>IoT Test Utility</t>
-  </si>
-  <si>
     <t>NetAgent</t>
   </si>
   <si>
     <t>NetShip</t>
   </si>
   <si>
-    <t>EDI - API/ FTP</t>
-  </si>
-  <si>
-    <t>MNXTracking</t>
-  </si>
-  <si>
-    <t>Mobile Application - Netship</t>
-  </si>
-  <si>
-    <t>Mobile Application - Agent</t>
-  </si>
-  <si>
-    <t>Tracking DashBoard</t>
-  </si>
-  <si>
-    <t>inbound/dashboard</t>
-  </si>
-  <si>
-    <t>CustomerCSVService</t>
-  </si>
-  <si>
-    <t>QualtexActiveOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fedex </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fedex Tracking </t>
-  </si>
-  <si>
-    <t>CR_27</t>
-  </si>
-  <si>
-    <t>SSRS Report</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -91,6 +38,75 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>http://10.20.104.71:8072/</t>
+  </si>
+  <si>
+    <t>Test Utility (Cheetah Order Processing)</t>
+  </si>
+  <si>
+    <t>http://10.20.104.71:9077/PublicServiceWebApplication/FlashWsV2.aspx</t>
+  </si>
+  <si>
+    <t>FedEx CIL/ MDSI</t>
+  </si>
+  <si>
+    <t>http://10.20.104.71:9077/TestApplicationUtility/</t>
+  </si>
+  <si>
+    <t>https://stagingna.nglog.com/login</t>
+  </si>
+  <si>
+    <t>https://stagingna.nglog.com/support</t>
+  </si>
+  <si>
+    <t>https://stagingns.nglog.com/</t>
+  </si>
+  <si>
+    <t>https://stagingns.nglog.com/support</t>
+  </si>
+  <si>
+    <t>https://staging.fedexsameday.com</t>
+  </si>
+  <si>
+    <t>Special Support - FedEx RW/ CR_46</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>testsamyak10</t>
+  </si>
+  <si>
+    <t>samyak10</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>samyakqa</t>
+  </si>
+  <si>
+    <t>DenverQA1</t>
+  </si>
+  <si>
+    <t>NetAgent Support Login</t>
+  </si>
+  <si>
+    <t>NetShip Support Login</t>
+  </si>
+  <si>
+    <t>tathya2</t>
+  </si>
+  <si>
+    <t>Tathya@2</t>
+  </si>
+  <si>
+    <t>https://staging.fedexsameday.com/specialsupport.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FedEX </t>
   </si>
 </sst>
 </file>
@@ -249,18 +265,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +407,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5F5"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -528,7 +541,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -571,33 +584,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -631,6 +645,7 @@
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -1006,212 +1021,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="67.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="22.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>34691</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
+        <v>950024</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="2"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://staging.fedexsameday.com/"/>
+    <hyperlink ref="D4" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FedEx All link file
</commit_message>
<xml_diff>
--- a/BrokenLink/src/main/resources/AllLinks_STG.xlsx
+++ b/BrokenLink/src/main/resources/AllLinks_STG.xlsx
@@ -106,7 +106,7 @@
     <t>https://staging.fedexsameday.com/specialsupport.aspx</t>
   </si>
   <si>
-    <t xml:space="preserve">FedEX </t>
+    <t>FedEXSameDay</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>